<commit_message>
increased clock division by factor 10, got a 1Hz-esque blink. Math is suspect and I'm not sure why this is. Warrants more investigation but I'll move on to the next exercise in the meantime.
</commit_message>
<xml_diff>
--- a/Exercise11p1-Interrupt_Blink/stm32 timer worksheet.xlsx
+++ b/Exercise11p1-Interrupt_Blink/stm32 timer worksheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\OneDrive\Documents\DiscoveringSTM32\Exercise11p1-Interrupt_Blink\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD0242EE-2FC9-44BD-B8D7-D27E68EE589B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1EB8032-60EA-4609-91F0-3EEC02A50038}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{3B03197A-48E6-4BCF-AE5C-62A4470EC6D8}"/>
   </bookViews>
@@ -78,7 +78,7 @@
     <t>input capture</t>
   </si>
   <si>
-    <t>LED blink</t>
+    <t>LED blink -this im not sure on</t>
   </si>
 </sst>
 </file>
@@ -554,7 +554,7 @@
         <v>1000000</v>
       </c>
       <c r="C3">
-        <f>$A$2/B3</f>
+        <f>A3/B3</f>
         <v>72</v>
       </c>
       <c r="D3">
@@ -586,30 +586,30 @@
         <v>72000000</v>
       </c>
       <c r="B4" s="2">
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="C4">
-        <f>$A$2/B4</f>
-        <v>72</v>
+        <f>A4/B4</f>
+        <v>720</v>
       </c>
       <c r="D4">
         <f>A4/C4</f>
-        <v>1000000</v>
+        <v>100000</v>
       </c>
       <c r="E4" s="3">
         <f>1/D4</f>
-        <v>9.9999999999999995E-7</v>
+        <v>1.0000000000000001E-5</v>
       </c>
       <c r="F4">
         <v>500000</v>
       </c>
       <c r="G4">
         <f>D4/F4</f>
-        <v>2</v>
+        <v>0.2</v>
       </c>
       <c r="H4">
         <f>1/G4</f>
-        <v>0.5</v>
+        <v>5</v>
       </c>
       <c r="J4" s="4"/>
       <c r="L4" t="s">

</xml_diff>